<commit_message>
Leg kick (minor changes)
Muscle properties loaded from xml file
ballandsocket joint is working but unstable. Controllers on free dof of ankle must be added
checked inertial and muscle properties
</commit_message>
<xml_diff>
--- a/DG_Tutorial_Newton/inertial_data.xlsx
+++ b/DG_Tutorial_Newton/inertial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\shaked_walker\DG_Tutorial_Newton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF46B33-4C02-4B25-B963-FF69DAB03DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3E8719-0940-4944-8240-2E59F4195299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12810" yWindow="720" windowWidth="13755" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final_model_values" sheetId="9" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="268">
   <si>
     <t>Segment</t>
   </si>
@@ -1167,15 +1167,6 @@
     <t>body mass/total mass [-]</t>
   </si>
   <si>
-    <t>Radii of gyration sagittal (Z)</t>
-  </si>
-  <si>
-    <t>Radii of gyration transverse (X)</t>
-  </si>
-  <si>
-    <t>Radii of gyration longitudinal (Y)</t>
-  </si>
-  <si>
     <t>Hip (half)</t>
   </si>
   <si>
@@ -1195,14 +1186,36 @@
   </si>
   <si>
     <t>UpArm</t>
+  </si>
+  <si>
+    <t>Izz kg*m^2</t>
+  </si>
+  <si>
+    <t>Ixx kg*m^2</t>
+  </si>
+  <si>
+    <t>Iyy kg*m^2</t>
+  </si>
+  <si>
+    <t>Radii of gyration sagittal % (Z)</t>
+  </si>
+  <si>
+    <t>Radii of gyration transverse % (X)</t>
+  </si>
+  <si>
+    <t>Radii of gyration longitudinal % (Y)</t>
+  </si>
+  <si>
+    <t>body mass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -1321,7 +1334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1352,8 +1365,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="47">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1653,37 +1672,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -1927,11 +1916,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2104,43 +2102,39 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2152,21 +2146,21 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2250,6 +2244,17 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -9628,13 +9633,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>697169</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>134432</xdr:rowOff>
@@ -9686,13 +9691,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>161926</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -9710,7 +9715,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3390900" y="3390900"/>
+          <a:off x="4095750" y="3390900"/>
           <a:ext cx="2867026" cy="1733550"/>
           <a:chOff x="4438650" y="3448050"/>
           <a:chExt cx="2079013" cy="1762125"/>
@@ -10040,7 +10045,7 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -10673,86 +10678,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8E0C8E-2076-4CAB-A2AC-06D6C11393CE}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:13" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="91" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="70" t="s">
         <v>242</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="F1" s="70" t="s">
         <v>253</v>
       </c>
-      <c r="F1" s="74" t="s">
-        <v>254</v>
-      </c>
-      <c r="G1" s="74" t="s">
-        <v>255</v>
-      </c>
-      <c r="H1" s="75" t="s">
-        <v>256</v>
-      </c>
+      <c r="G1" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H1" s="70" t="s">
+        <v>265</v>
+      </c>
+      <c r="I1" s="71" t="s">
+        <v>266</v>
+      </c>
+      <c r="J1" s="124" t="s">
+        <v>261</v>
+      </c>
+      <c r="K1" s="124" t="s">
+        <v>262</v>
+      </c>
+      <c r="L1" s="124" t="s">
+        <v>263</v>
+      </c>
+      <c r="M1" s="126"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="96">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="92">
         <v>0</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="72">
+      <c r="C2" s="69">
         <f>'Leva Wang inertia calculation'!F2</f>
         <v>0.20330000000000001</v>
       </c>
-      <c r="D2" s="72">
+      <c r="D2" s="69">
         <v>0.6</v>
       </c>
-      <c r="E2" s="72">
+      <c r="E2" s="69">
+        <f>F2*$C$21</f>
+        <v>5.0662000000000003</v>
+      </c>
+      <c r="F2" s="69">
         <f>'Leva Wang inertia calculation'!B2/100</f>
         <v>6.9400000000000003E-2</v>
       </c>
-      <c r="F2" s="72">
-        <f>'Leva Wang inertia calculation'!B2/100</f>
-        <v>6.9400000000000003E-2</v>
-      </c>
-      <c r="G2" s="72">
-        <f>'Leva Wang inertia calculation'!C2/100</f>
+      <c r="G2" s="127">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="H2" s="127">
+        <v>0.376</v>
+      </c>
+      <c r="I2" s="128">
         <v>0.312</v>
       </c>
-      <c r="H2" s="73">
-        <f>'Leva Wang inertia calculation'!D2/100</f>
-        <v>0.36200000000000004</v>
+      <c r="J2" s="13">
+        <f>(G2*$C2)^2*$F2*$C$21</f>
+        <v>2.7439375878674389E-2</v>
+      </c>
+      <c r="K2" s="13">
+        <f>(H2*$C2)^2*$F2*$C$21</f>
+        <v>2.9602799092087174E-2</v>
+      </c>
+      <c r="L2" s="13">
+        <f>(I2*$C2)^2*$F2*$C$21</f>
+        <v>2.0382914177937791E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="97">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="93">
         <v>1</v>
       </c>
-      <c r="B3" s="92" t="s">
-        <v>263</v>
+      <c r="B3" s="88" t="s">
+        <v>260</v>
       </c>
       <c r="C3" s="63">
         <f>'Leva Wang inertia calculation'!F3</f>
@@ -10761,28 +10794,41 @@
       <c r="D3" s="63">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E3" s="63">
-        <f>'Leva Wang inertia calculation'!B3/100</f>
-        <v>2.7099999999999999E-2</v>
+      <c r="E3" s="69">
+        <f t="shared" ref="E3:E13" si="0">F3*$C$21</f>
+        <v>1.9782999999999999</v>
       </c>
       <c r="F3" s="63">
         <f>'Leva Wang inertia calculation'!B3/100</f>
         <v>2.7099999999999999E-2</v>
       </c>
-      <c r="G3" s="63">
-        <f>'Leva Wang inertia calculation'!C3/100</f>
+      <c r="G3" s="127">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="H3" s="127">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="I3" s="128">
         <v>0.158</v>
       </c>
-      <c r="H3" s="66">
-        <f>'Leva Wang inertia calculation'!D3/100</f>
-        <v>0.28499999999999998</v>
+      <c r="J3" s="13">
+        <f>(G3*$C3)^2*$F3*$C$21</f>
+        <v>1.2751332340096575E-2</v>
+      </c>
+      <c r="K3" s="13">
+        <f>(H3*$C3)^2*$F3*$C$21</f>
+        <v>1.1359792668042207E-2</v>
+      </c>
+      <c r="L3" s="13">
+        <f>(I3*$C3)^2*$F3*$C$21</f>
+        <v>3.9190429121350682E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="96">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="92">
         <v>2</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="88" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="63">
@@ -10792,28 +10838,41 @@
       <c r="D4" s="63">
         <v>0.46</v>
       </c>
-      <c r="E4" s="63">
-        <f>'Leva Wang inertia calculation'!B4/100</f>
-        <v>1.6200000000000003E-2</v>
+      <c r="E4" s="69">
+        <f t="shared" si="0"/>
+        <v>1.1826000000000001</v>
       </c>
       <c r="F4" s="63">
         <f>'Leva Wang inertia calculation'!B4/100</f>
         <v>1.6200000000000003E-2</v>
       </c>
-      <c r="G4" s="63">
-        <f>'Leva Wang inertia calculation'!C4/100</f>
+      <c r="G4" s="127">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="H4" s="127">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="I4" s="128">
         <v>0.121</v>
       </c>
-      <c r="H4" s="66">
-        <f>'Leva Wang inertia calculation'!D4/100</f>
-        <v>0.27600000000000002</v>
+      <c r="J4" s="13">
+        <f>(G4*$C4)^2*$F4*$C$21</f>
+        <v>6.5138483466480974E-3</v>
+      </c>
+      <c r="K4" s="13">
+        <f>(H4*$C4)^2*$F4*$C$21</f>
+        <v>6.0049753221928523E-3</v>
+      </c>
+      <c r="L4" s="13">
+        <f>(I4*$C4)^2*$F4*$C$21</f>
+        <v>1.2519593263399858E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="97">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="93">
         <v>3</v>
       </c>
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="88" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="63">
@@ -10823,28 +10882,41 @@
       <c r="D5" s="63">
         <v>0.79</v>
       </c>
-      <c r="E5" s="63">
+      <c r="E5" s="130">
+        <f t="shared" si="0"/>
+        <v>0.44529999999999997</v>
+      </c>
+      <c r="F5" s="129">
         <f>'Leva Wang inertia calculation'!B5/100</f>
         <v>6.0999999999999995E-3</v>
       </c>
-      <c r="F5" s="63">
-        <f>'Leva Wang inertia calculation'!B5/100</f>
-        <v>6.0999999999999995E-3</v>
-      </c>
-      <c r="G5" s="63">
-        <f>'Leva Wang inertia calculation'!C5/100</f>
+      <c r="G5" s="127">
+        <v>0.628</v>
+      </c>
+      <c r="H5" s="127">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="I5" s="128">
         <v>0.40100000000000002</v>
       </c>
-      <c r="H5" s="66">
-        <f>'Leva Wang inertia calculation'!D5/100</f>
-        <v>0.628</v>
+      <c r="J5" s="13">
+        <f>(G5*$C5)^2*$F5*$C$21</f>
+        <v>1.3049278927818879E-3</v>
+      </c>
+      <c r="K5" s="13">
+        <f>(H5*$C5)^2*$F5*$C$21</f>
+        <v>8.7076699007950799E-4</v>
+      </c>
+      <c r="L5" s="13">
+        <f>(I5*$C5)^2*$F5*$C$21</f>
+        <v>5.320543178405319E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="96">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="92">
         <v>4</v>
       </c>
-      <c r="B6" s="92" t="s">
+      <c r="B6" s="88" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="63">
@@ -10854,28 +10926,41 @@
       <c r="D6" s="63">
         <v>0.45</v>
       </c>
-      <c r="E6" s="63">
-        <f>'Leva Wang inertia calculation'!B6/100</f>
-        <v>0.43459999999999999</v>
+      <c r="E6" s="69">
+        <f t="shared" si="0"/>
+        <v>31.7258</v>
       </c>
       <c r="F6" s="63">
         <f>'Leva Wang inertia calculation'!B6/100</f>
         <v>0.43459999999999999</v>
       </c>
-      <c r="G6" s="63">
-        <f>'Leva Wang inertia calculation'!C6/100</f>
+      <c r="G6" s="127">
+        <v>0.372</v>
+      </c>
+      <c r="H6" s="127">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="I6" s="128">
         <v>0.191</v>
       </c>
-      <c r="H6" s="66">
-        <f>'Leva Wang inertia calculation'!D6/100</f>
-        <v>0.37200000000000005</v>
+      <c r="J6" s="13">
+        <f>(G6*$C6)^2*$F6*$C$21</f>
+        <v>1.242105378968998</v>
+      </c>
+      <c r="K6" s="13">
+        <f>(H6*$C6)^2*$F6*$C$21</f>
+        <v>1.0807655984526969</v>
+      </c>
+      <c r="L6" s="13">
+        <f>(I6*$C6)^2*$F6*$C$21</f>
+        <v>0.32744570420112162</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="97">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="93">
         <v>5</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="88" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="63">
@@ -10885,28 +10970,44 @@
       <c r="D7" s="63">
         <v>0.41</v>
       </c>
-      <c r="E7" s="63">
-        <f>'Leva Wang inertia calculation'!B7/100</f>
-        <v>0.1416</v>
+      <c r="E7" s="69">
+        <f t="shared" si="0"/>
+        <v>10.3368</v>
       </c>
       <c r="F7" s="63">
         <f>'Leva Wang inertia calculation'!B7/100</f>
         <v>0.1416</v>
       </c>
-      <c r="G7" s="63">
+      <c r="G7" s="127">
         <f>'Leva Wang inertia calculation'!C7/100</f>
         <v>0.14899999999999999</v>
       </c>
-      <c r="H7" s="66">
+      <c r="H7" s="127">
         <f>'Leva Wang inertia calculation'!D7/100</f>
         <v>0.32899999999999996</v>
       </c>
+      <c r="I7" s="128">
+        <f>'Leva Wang inertia calculation'!E7/100</f>
+        <v>0.32899999999999996</v>
+      </c>
+      <c r="J7" s="13">
+        <f>(G7*$C7)^2*$F7*$C$21</f>
+        <v>4.0906762398522908E-2</v>
+      </c>
+      <c r="K7" s="13">
+        <f>(H7*$C7)^2*$F7*$C$21</f>
+        <v>0.19944096521681537</v>
+      </c>
+      <c r="L7" s="13">
+        <f>(I7*$C7)^2*$F7*$C$21</f>
+        <v>0.19944096521681537</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="96">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="92">
         <v>6</v>
       </c>
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="88" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="63">
@@ -10916,28 +11017,44 @@
       <c r="D8" s="63">
         <v>0.45</v>
       </c>
-      <c r="E8" s="63">
-        <f>'Leva Wang inertia calculation'!B8/100</f>
-        <v>4.3299999999999998E-2</v>
+      <c r="E8" s="69">
+        <f t="shared" si="0"/>
+        <v>3.1608999999999998</v>
       </c>
       <c r="F8" s="63">
         <f>'Leva Wang inertia calculation'!B8/100</f>
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="G8" s="63">
+      <c r="G8" s="127">
         <f>'Leva Wang inertia calculation'!C8/100</f>
         <v>0.10300000000000001</v>
       </c>
-      <c r="H8" s="66">
+      <c r="H8" s="127">
         <f>'Leva Wang inertia calculation'!D8/100</f>
         <v>0.255</v>
       </c>
+      <c r="I8" s="128">
+        <f>'Leva Wang inertia calculation'!E8/100</f>
+        <v>0.249</v>
+      </c>
+      <c r="J8" s="13">
+        <f>(G8*$C8)^2*$F8*$C$21</f>
+        <v>6.3163278625636013E-3</v>
+      </c>
+      <c r="K8" s="13">
+        <f>(H8*$C8)^2*$F8*$C$21</f>
+        <v>3.871422558801E-2</v>
+      </c>
+      <c r="L8" s="13">
+        <f>(I8*$C8)^2*$F8*$C$21</f>
+        <v>3.6913813159280398E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="97">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="93">
         <v>7</v>
       </c>
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="88" t="s">
         <v>139</v>
       </c>
       <c r="C9" s="63">
@@ -10947,28 +11064,41 @@
       <c r="D9" s="63">
         <v>0.44</v>
       </c>
-      <c r="E9" s="63">
-        <f>'Leva Wang inertia calculation'!B9/100</f>
-        <v>1.37E-2</v>
+      <c r="E9" s="69">
+        <f t="shared" si="0"/>
+        <v>1.0001</v>
       </c>
       <c r="F9" s="63">
         <f>'Leva Wang inertia calculation'!B9/100</f>
         <v>1.37E-2</v>
       </c>
-      <c r="G9" s="63">
-        <f>'Leva Wang inertia calculation'!C9/100</f>
+      <c r="G9" s="127">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="H9" s="127">
+        <v>0.245</v>
+      </c>
+      <c r="I9" s="128">
         <v>0.124</v>
       </c>
-      <c r="H9" s="66">
-        <f>'Leva Wang inertia calculation'!D9/100</f>
-        <v>0.25700000000000001</v>
+      <c r="J9" s="13">
+        <f>(G9*$C9)^2*$F9*$C$21</f>
+        <v>4.4003344143324899E-3</v>
+      </c>
+      <c r="K9" s="13">
+        <f>(H9*$C9)^2*$F9*$C$21</f>
+        <v>3.9990018504490249E-3</v>
+      </c>
+      <c r="L9" s="13">
+        <f>(I9*$C9)^2*$F9*$C$21</f>
+        <v>1.0243840475219362E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="96">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="92">
         <v>8</v>
       </c>
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="89" t="s">
         <v>248</v>
       </c>
       <c r="C10" s="64">
@@ -10978,29 +11108,45 @@
       <c r="D10" s="63">
         <v>0.5</v>
       </c>
-      <c r="E10" s="63">
+      <c r="E10" s="69">
+        <f t="shared" si="0"/>
+        <v>0.18872900000000001</v>
+      </c>
+      <c r="F10" s="63">
         <f>'wang inertia mass COM'!H17/C21</f>
         <v>2.5853287671232877E-3</v>
       </c>
-      <c r="F10" s="63">
-        <f>SQRT('wang inertia mass COM'!D18/(E10*C21))</f>
-        <v>3.0363742851808498E-2</v>
-      </c>
-      <c r="G10" s="63">
-        <f>SQRT('wang inertia mass COM'!B18/(E10*C21))</f>
-        <v>2.1482744244188664E-2</v>
-      </c>
-      <c r="H10" s="66">
-        <f>SQRT('wang inertia mass COM'!C18/(E10*C21))</f>
-        <v>6.793440220250864E-2</v>
+      <c r="G10" s="127">
+        <f>SQRT(J10/F10/$C$21)/$C10</f>
+        <v>0.45291668587005951</v>
+      </c>
+      <c r="H10" s="127">
+        <f>SQRT(K10/F10/$C$21)/$C10</f>
+        <v>1.4322483176443885</v>
+      </c>
+      <c r="I10" s="127">
+        <f>SQRT(L10/F10/$C$21)/$C10</f>
+        <v>0.64015312134863589</v>
+      </c>
+      <c r="J10" s="125">
+        <f>'wang inertia mass COM'!B17</f>
+        <v>8.7100000000000003E-5</v>
+      </c>
+      <c r="K10" s="125">
+        <f>'wang inertia mass COM'!C17</f>
+        <v>8.7100000000000003E-4</v>
+      </c>
+      <c r="L10" s="125">
+        <f>'wang inertia mass COM'!D17</f>
+        <v>1.74E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="97">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="93">
         <v>9</v>
       </c>
-      <c r="B11" s="92" t="s">
-        <v>258</v>
+      <c r="B11" s="88" t="s">
+        <v>255</v>
       </c>
       <c r="C11" s="64">
         <v>0.17069999999999999</v>
@@ -11009,29 +11155,42 @@
         <f>29.99/100</f>
         <v>0.2999</v>
       </c>
-      <c r="E11" s="65">
+      <c r="E11" s="69">
+        <f t="shared" si="0"/>
+        <v>15.96</v>
+      </c>
+      <c r="F11" s="65">
         <f>15.96/C21</f>
         <v>0.21863013698630138</v>
       </c>
-      <c r="F11" s="64">
-        <f>71.6/100</f>
+      <c r="G11" s="127">
         <v>0.71599999999999997</v>
       </c>
-      <c r="G11" s="64">
-        <f>45.4/100</f>
-        <v>0.45399999999999996</v>
-      </c>
-      <c r="H11" s="67">
-        <f>65.9/100</f>
+      <c r="H11" s="127">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="I11" s="128">
         <v>0.65900000000000003</v>
       </c>
+      <c r="J11" s="13">
+        <f>(G11*$C11)^2*$F11*$C$21</f>
+        <v>0.23841082680186235</v>
+      </c>
+      <c r="K11" s="13">
+        <f>(H11*$C11)^2*$F11*$C$21</f>
+        <v>9.5854307717246387E-2</v>
+      </c>
+      <c r="L11" s="13">
+        <f>(I11*$C11)^2*$F11*$C$21</f>
+        <v>0.20196250950801242</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="96">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="92">
         <v>10</v>
       </c>
-      <c r="B12" s="92" t="s">
-        <v>259</v>
+      <c r="B12" s="88" t="s">
+        <v>256</v>
       </c>
       <c r="C12" s="64">
         <f>215.5/1000</f>
@@ -11041,90 +11200,117 @@
         <f>45.02/100</f>
         <v>0.45020000000000004</v>
       </c>
-      <c r="E12" s="65">
+      <c r="E12" s="69">
+        <f t="shared" si="0"/>
+        <v>16.329999999999998</v>
+      </c>
+      <c r="F12" s="65">
         <f>16.33/C21</f>
         <v>0.22369863013698627</v>
       </c>
-      <c r="F12" s="64">
-        <f>48.2/100</f>
-        <v>0.48200000000000004</v>
-      </c>
-      <c r="G12" s="64">
-        <f>38.3/100</f>
-        <v>0.38299999999999995</v>
-      </c>
-      <c r="H12" s="67">
-        <f>46.8/100</f>
-        <v>0.46799999999999997</v>
+      <c r="G12" s="127">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="H12" s="127">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="I12" s="128">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="J12" s="13">
+        <f>(G12*$C12)^2*$F12*$C$21</f>
+        <v>0.17618738518752997</v>
+      </c>
+      <c r="K12" s="13">
+        <f>(H12*$C12)^2*$F12*$C$21</f>
+        <v>0.11124443168064248</v>
+      </c>
+      <c r="L12" s="13">
+        <f>(I12*$C12)^2*$F12*$C$21</f>
+        <v>0.16681166574798245</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="97">
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="93">
         <v>11</v>
       </c>
-      <c r="B13" s="94" t="s">
-        <v>260</v>
-      </c>
-      <c r="C13" s="68">
+      <c r="B13" s="90" t="s">
+        <v>257</v>
+      </c>
+      <c r="C13" s="66">
         <f>145.7/1000</f>
         <v>0.1457</v>
       </c>
-      <c r="D13" s="69">
+      <c r="D13" s="67">
         <f>61.15/100</f>
         <v>0.61149999999999993</v>
       </c>
-      <c r="E13" s="70">
+      <c r="E13" s="69">
+        <f t="shared" si="0"/>
+        <v>11.17</v>
+      </c>
+      <c r="F13" s="68">
         <f>11.17/C21</f>
         <v>0.15301369863013697</v>
       </c>
-      <c r="F13" s="70">
-        <f>61.5/100</f>
+      <c r="G13" s="127">
         <v>0.61499999999999999</v>
       </c>
-      <c r="G13" s="70">
-        <f>55.1/100</f>
+      <c r="H13" s="127">
         <v>0.55100000000000005</v>
       </c>
-      <c r="H13" s="71">
-        <f>58.7/100</f>
-        <v>0.58700000000000008</v>
-      </c>
-      <c r="I13" s="62"/>
+      <c r="I13" s="128">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="J13" s="13">
+        <f>(G13*$C13)^2*$F13*$C$21</f>
+        <v>8.9685556689892476E-2</v>
+      </c>
+      <c r="K13" s="13">
+        <f>(H13*$C13)^2*$F13*$C$21</f>
+        <v>7.1990547152113324E-2</v>
+      </c>
+      <c r="L13" s="13">
+        <f>(I13*$C13)^2*$F13*$C$21</f>
+        <v>5.1935460026299202E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="57"/>
       <c r="B14" s="61"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="59"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="59"/>
       <c r="H14" s="59"/>
-      <c r="I14" s="62"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="62"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="86" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="82" t="s">
         <v>239</v>
       </c>
-      <c r="B15" s="99" t="s">
-        <v>261</v>
-      </c>
-      <c r="C15" s="100"/>
+      <c r="B15" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" s="96"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="59"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="60"/>
       <c r="G15" s="59"/>
       <c r="H15" s="59"/>
-      <c r="I15" s="62"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="62"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="87">
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="83">
         <v>12</v>
       </c>
-      <c r="B16" s="76" t="s">
-        <v>257</v>
-      </c>
-      <c r="C16" s="77">
+      <c r="B16" s="72" t="s">
+        <v>254</v>
+      </c>
+      <c r="C16" s="73">
         <f>0.191*C22/2</f>
         <v>0.16626550000000001</v>
       </c>
@@ -11135,131 +11321,133 @@
       <c r="F16" s="56"/>
       <c r="G16" s="56"/>
       <c r="H16" s="56"/>
-      <c r="I16" s="62"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="62"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="87">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="83">
         <v>13</v>
       </c>
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="74" t="s">
         <v>249</v>
       </c>
-      <c r="C17" s="79">
+      <c r="C17" s="75">
         <f>0.259*C22/2</f>
         <v>0.22545950000000001</v>
       </c>
       <c r="D17" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="E17" s="58"/>
-      <c r="F17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="58"/>
       <c r="G17" s="56"/>
       <c r="H17" s="56"/>
-      <c r="I17" s="101" t="s">
+      <c r="I17" s="56"/>
+      <c r="J17" s="97" t="s">
         <v>250</v>
       </c>
-      <c r="J17" s="102"/>
-      <c r="K17" s="103"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="99"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="87">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="83">
         <v>14</v>
       </c>
-      <c r="B18" s="78" t="s">
+      <c r="B18" s="74" t="s">
         <v>245</v>
       </c>
-      <c r="C18" s="79">
+      <c r="C18" s="75">
         <f>0.055*C22</f>
         <v>9.5755000000000007E-2</v>
       </c>
       <c r="D18" t="s">
         <v>244</v>
       </c>
-      <c r="I18" s="104" t="s">
+      <c r="J18" s="100" t="s">
         <v>240</v>
       </c>
-      <c r="J18" s="105"/>
-      <c r="K18" s="106"/>
+      <c r="K18" s="101"/>
+      <c r="L18" s="102"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="87">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="83">
         <v>15</v>
       </c>
-      <c r="B19" s="78" t="s">
+      <c r="B19" s="74" t="s">
         <v>246</v>
       </c>
-      <c r="C19" s="79">
+      <c r="C19" s="75">
         <f>0.039*C22</f>
         <v>6.7899000000000001E-2</v>
       </c>
       <c r="D19" t="s">
         <v>244</v>
       </c>
-      <c r="I19" s="107" t="s">
+      <c r="J19" s="103" t="s">
         <v>241</v>
       </c>
-      <c r="J19" s="108"/>
-      <c r="K19" s="109"/>
+      <c r="K19" s="104"/>
+      <c r="L19" s="105"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="87">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="83">
         <v>16</v>
       </c>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="76" t="s">
         <v>220</v>
       </c>
-      <c r="C20" s="81">
+      <c r="C20" s="77">
         <f>0.0396</f>
         <v>3.9600000000000003E-2</v>
       </c>
       <c r="D20" t="s">
-        <v>262</v>
-      </c>
-      <c r="I20" s="110" t="s">
+        <v>259</v>
+      </c>
+      <c r="J20" s="106" t="s">
         <v>247</v>
       </c>
-      <c r="J20" s="111"/>
-      <c r="K20" s="112"/>
+      <c r="K20" s="107"/>
+      <c r="L20" s="108"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="88"/>
-      <c r="B21" s="82" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="84"/>
+      <c r="B21" s="78" t="s">
         <v>251</v>
       </c>
-      <c r="C21" s="83">
+      <c r="C21" s="79">
         <v>73</v>
       </c>
       <c r="D21" t="s">
         <v>252</v>
       </c>
-      <c r="I21" s="98"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="98"/>
-      <c r="L21" s="20"/>
+      <c r="J21" s="94"/>
+      <c r="K21" s="94"/>
+      <c r="L21" s="94"/>
+      <c r="M21" s="20"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="89"/>
-      <c r="B22" s="84" t="s">
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="85"/>
+      <c r="B22" s="80" t="s">
         <v>243</v>
       </c>
-      <c r="C22" s="85">
+      <c r="C22" s="81">
         <v>1.7410000000000001</v>
       </c>
       <c r="D22" t="s">
         <v>244</v>
       </c>
-      <c r="I22" s="20"/>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="J21:L21"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11272,7 +11460,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11858,17 +12046,17 @@
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
-      <c r="N10" s="113" t="s">
+      <c r="N10" s="109" t="s">
         <v>119</v>
       </c>
-      <c r="O10" s="113"/>
-      <c r="P10" s="113"/>
-      <c r="Q10" s="113"/>
-      <c r="S10" s="115" t="s">
+      <c r="O10" s="109"/>
+      <c r="P10" s="109"/>
+      <c r="Q10" s="109"/>
+      <c r="S10" s="111" t="s">
         <v>121</v>
       </c>
-      <c r="T10" s="115"/>
-      <c r="U10" s="115"/>
+      <c r="T10" s="111"/>
+      <c r="U10" s="111"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
@@ -11910,19 +12098,19 @@
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="114" t="s">
+      <c r="A13" s="110" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="114"/>
-      <c r="C13" s="114"/>
-      <c r="D13" s="114"/>
-      <c r="E13" s="114"/>
-      <c r="F13" s="114"/>
-      <c r="G13" s="114"/>
-      <c r="H13" s="114"/>
-      <c r="I13" s="114"/>
-      <c r="J13" s="114"/>
-      <c r="K13" s="114"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="110"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="N16" s="22"/>
@@ -11959,8 +12147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03B814C-BB95-4898-AEF0-165F4CD8FBE0}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35:F37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12604,7 +12792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF30069-4F66-4BA4-904C-6A03E4672BD3}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -14042,8 +14230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F9D47B6-DDD1-434A-9B8A-4E64BB263848}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14055,10 +14243,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="115" t="s">
         <v>122</v>
       </c>
       <c r="C1" s="29" t="s">
@@ -14073,8 +14261,8 @@
       <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="117"/>
-      <c r="B2" s="120"/>
+      <c r="A2" s="113"/>
+      <c r="B2" s="116"/>
       <c r="C2" s="32" t="s">
         <v>126</v>
       </c>
@@ -14089,8 +14277,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="117"/>
-      <c r="B3" s="120"/>
+      <c r="A3" s="113"/>
+      <c r="B3" s="116"/>
       <c r="C3" s="32" t="s">
         <v>130</v>
       </c>
@@ -14105,8 +14293,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="118"/>
-      <c r="B4" s="121"/>
+      <c r="A4" s="114"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="35" t="s">
         <v>131</v>
       </c>
@@ -14342,16 +14530,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45"/>
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="118" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="124"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="120"/>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="121" t="s">
         <v>144</v>
       </c>
       <c r="B2" s="46" t="s">
@@ -14371,7 +14559,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="126"/>
+      <c r="A3" s="122"/>
       <c r="B3" s="48" t="s">
         <v>150</v>
       </c>
@@ -14576,30 +14764,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="123" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="C1" s="127" t="s">
+      <c r="C1" s="123" t="s">
         <v>236</v>
       </c>
-      <c r="D1" s="127" t="s">
+      <c r="D1" s="123" t="s">
         <v>235</v>
       </c>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127" t="s">
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="127"/>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
+      <c r="A2" s="123"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
       <c r="D2" s="55" t="s">
         <v>233</v>
       </c>

</xml_diff>